<commit_message>
2023 July 13 09:49am
</commit_message>
<xml_diff>
--- a/Models/Fed Models/correlations fed.xlsx
+++ b/Models/Fed Models/correlations fed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -458,13 +458,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.526</v>
+        <v>0.5336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -473,13 +473,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5083</v>
+        <v>0.526</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
@@ -488,13 +488,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5947</v>
+        <v>0.5083</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>mortgage</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5641</v>
+        <v>0.5947</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>recession</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -518,21 +518,6 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5054</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>trade</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>Frequency</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
         <v>0.3426</v>
       </c>
     </row>

</xml_diff>